<commit_message>
spar & picknpay csv
</commit_message>
<xml_diff>
--- a/Choppies.xlsx
+++ b/Choppies.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Choppies" sheetId="1" r:id="rId1"/>
     <sheet name="payless" sheetId="3" r:id="rId2"/>
-    <sheet name="shoprite" sheetId="2" r:id="rId3"/>
+    <sheet name="Pick n Pay" sheetId="4" r:id="rId3"/>
+    <sheet name="shoprite" sheetId="2" r:id="rId4"/>
+    <sheet name="Spar" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Choppies!$C$1:$C$109</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="395">
   <si>
     <t>Name</t>
   </si>
@@ -917,13 +919,310 @@
   </si>
   <si>
     <t>Kgalagadi</t>
+  </si>
+  <si>
+    <t>Pick N Pay Botswana</t>
+  </si>
+  <si>
+    <t>Plot 1277, Clover House, Old Lobatse Road</t>
+  </si>
+  <si>
+    <t>Pick N Pay Family Supermarket Dairy</t>
+  </si>
+  <si>
+    <t>Shop 1 Dairy Site, Southring Mall Extension 12, Gaborone</t>
+  </si>
+  <si>
+    <t>Pick N Pay Family Supermarket Francistown 2</t>
+  </si>
+  <si>
+    <t>Plot 839-840/841-846, Blue Jacket Street, Francistown</t>
+  </si>
+  <si>
+    <t>Pick N Pay Jwaneng</t>
+  </si>
+  <si>
+    <t>Plot 5415, Jwaneng Mall, Teemane Avenue, Jwaneng</t>
+  </si>
+  <si>
+    <t>Pick N Pay Lobatse</t>
+  </si>
+  <si>
+    <t>Plot 1277, Old Lobatse Road, Gaborone</t>
+  </si>
+  <si>
+    <t>Pick N Pay Sebele</t>
+  </si>
+  <si>
+    <t>Sebele</t>
+  </si>
+  <si>
+    <t>Pick N Pay Selibe-Phikwe</t>
+  </si>
+  <si>
+    <t>Plot 6568, Tshekedi Road, Selibe Phikwe</t>
+  </si>
+  <si>
+    <t>Pick N Pay Family Supermarket Francistown 1</t>
+  </si>
+  <si>
+    <t>Pick N Pay Riverwalk</t>
+  </si>
+  <si>
+    <t>Pick N Pay Maun</t>
+  </si>
+  <si>
+    <t>Pick N Pay Molapo Crossing</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>54483, Unit 9, Molapo Crossing, Gaborone</t>
+  </si>
+  <si>
+    <t>Pick N Pay Hillside</t>
+  </si>
+  <si>
+    <t>Hillside Shopping Center</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Sebele Mall, A1</t>
+  </si>
+  <si>
+    <t>Shop No: 12, Riverwalk Mall, The Village Gaborone</t>
+  </si>
+  <si>
+    <t>1/112001</t>
+  </si>
+  <si>
+    <t>Cnr guy and, St Patrick St, Francistown</t>
+  </si>
+  <si>
+    <t>Shoprite Checkers</t>
+  </si>
+  <si>
+    <t>Airport junction, A1</t>
+  </si>
+  <si>
+    <t>Acacia Superspar</t>
+  </si>
+  <si>
+    <t>Plot 75123, Acacia Mall, Phakalane</t>
+  </si>
+  <si>
+    <t>Airport Junction Spar</t>
+  </si>
+  <si>
+    <t>Plot 70665, Shop 19 Airport Junction</t>
+  </si>
+  <si>
+    <t>Bamangwato Spar</t>
+  </si>
+  <si>
+    <t>Plot 1707, Unit No.8 Lobatse Complex, Palapye</t>
+  </si>
+  <si>
+    <t>Boiteko Junction Spar</t>
+  </si>
+  <si>
+    <t>Plot 2461, Boiteko Junction, Serowe</t>
+  </si>
+  <si>
+    <t>Boseja Spar</t>
+  </si>
+  <si>
+    <t>Plot 43094, Boseja Ward, Maun</t>
+  </si>
+  <si>
+    <t>Cbd Spar</t>
+  </si>
+  <si>
+    <t>Co-Op Spar</t>
+  </si>
+  <si>
+    <t>Lot 54381, The Square New Cental Business District, Gaborone</t>
+  </si>
+  <si>
+    <t>Plot 1109 -114, Main Mall, Gaborone,</t>
+  </si>
+  <si>
+    <t>Francistown Spar</t>
+  </si>
+  <si>
+    <t>Plot 904, Unit 10 &amp; 11, Nzano Shopping Centre, Francistown</t>
+  </si>
+  <si>
+    <t>G-West Spar</t>
+  </si>
+  <si>
+    <t>G-West Shopping Center, Gaborone West Phase 1, Gaborone</t>
+  </si>
+  <si>
+    <t>Ghanzi Spar</t>
+  </si>
+  <si>
+    <t>Plot 29, Ghanzi</t>
+  </si>
+  <si>
+    <t>Kanye Spar</t>
+  </si>
+  <si>
+    <t>Tribul Lot 6602, Mongala Mall, Kanye</t>
+  </si>
+  <si>
+    <t>Kasane Spar</t>
+  </si>
+  <si>
+    <t>Plot 2208, Unit 6 Hunters Africa, Kasane</t>
+  </si>
+  <si>
+    <t>Kgabo Spar</t>
+  </si>
+  <si>
+    <t>Plot 2985 Kgabo Mall Shopping Center, Phaphane, Mochud</t>
+  </si>
+  <si>
+    <t>Kgale Spar</t>
+  </si>
+  <si>
+    <t>Area 388 - Ko, Farm Forest Hill No9 - Ko Kgale, Gaborone</t>
+  </si>
+  <si>
+    <t>Kwena Spar</t>
+  </si>
+  <si>
+    <t>Plot 1359, Kwena Mall, Mogoditshane</t>
+  </si>
+  <si>
+    <t>Kweneng Spar</t>
+  </si>
+  <si>
+    <t>Plot 25917, Shop No.7, Turnrite Shopping Centre, Tsolamosese, Mogoditshane,</t>
+  </si>
+  <si>
+    <t>Letlhakane Spar</t>
+  </si>
+  <si>
+    <t>Tawana Ward Letlhakane Shopping Centre, Letlhakane</t>
+  </si>
+  <si>
+    <t>Lobatse Spar</t>
+  </si>
+  <si>
+    <t>Plot 14076, Peleng Ward, Lobatse</t>
+  </si>
+  <si>
+    <t>Mafenyatlala Spar</t>
+  </si>
+  <si>
+    <t>Plot 39, Shop 21 Mafenyatlala Mall, Molepolole</t>
+  </si>
+  <si>
+    <t>Mahalapye Spar</t>
+  </si>
+  <si>
+    <t>Plot 779 And 1082 Main Mall, Tshosa 2, Mahalapye</t>
+  </si>
+  <si>
+    <t>Main Mall Spar</t>
+  </si>
+  <si>
+    <t>Plots 799 And 1082, Main Mall, Mahalapye</t>
+  </si>
+  <si>
+    <t>Marang Spar</t>
+  </si>
+  <si>
+    <t>Plot 32397, Golden Valley Complex, Francistown</t>
+  </si>
+  <si>
+    <t>Molepolole Spar</t>
+  </si>
+  <si>
+    <t>Plot 1722, Molepolole</t>
+  </si>
+  <si>
+    <t>Nswazwi Spar</t>
+  </si>
+  <si>
+    <t>Plot 16177 - 161185, Nswazwi Mall Blue Jacket Street, Francistown</t>
+  </si>
+  <si>
+    <t>Orapa Spar</t>
+  </si>
+  <si>
+    <t>Sable Avenue, Orapa</t>
+  </si>
+  <si>
+    <t>Palapye Junction Spar</t>
+  </si>
+  <si>
+    <t>Plot 27737, Palapye Junction Shopping Centre, Palapye</t>
+  </si>
+  <si>
+    <t>Palapye Spar</t>
+  </si>
+  <si>
+    <t>Plot 68, Shop No.11, Palapye Mall, Palapye</t>
+  </si>
+  <si>
+    <t>Pula Spar</t>
+  </si>
+  <si>
+    <t>Plot 54502, Block 6, Gaborone</t>
+  </si>
+  <si>
+    <t>Rail Park Spar</t>
+  </si>
+  <si>
+    <t>Plot 4716, Shop G35, Rail Park Mall, Gaborone</t>
+  </si>
+  <si>
+    <t>Serowe Spar</t>
+  </si>
+  <si>
+    <t>Plot 3831, Main Mall, Serowe</t>
+  </si>
+  <si>
+    <t>Tlokweng Road Spar</t>
+  </si>
+  <si>
+    <t>Tswana Spar</t>
+  </si>
+  <si>
+    <t>Plot 27332, Block 3, Gaborone</t>
+  </si>
+  <si>
+    <t>Tutume Spar</t>
+  </si>
+  <si>
+    <t>Plot 2085, Mojanaga Shopping Complex Madikwe Ward, Tutume</t>
+  </si>
+  <si>
+    <t>Orapa</t>
+  </si>
+  <si>
+    <t>Sount-East</t>
+  </si>
+  <si>
+    <t>Plot 25117, Shop 5 Extension 15, Tlokweng Road, Riverwalk, Gaborone</t>
+  </si>
+  <si>
+    <t>Plot 2908, Rammopyana Ward, Mochudi</t>
+  </si>
+  <si>
+    <t>Mochudi Spar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -960,6 +1259,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF595A5B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595A5B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -994,7 +1305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1021,6 +1332,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1304,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3972,10 +4287,366 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2" s="23">
+        <v>40063</v>
+      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3">
+        <v>-24.6662479830552</v>
+      </c>
+      <c r="F3">
+        <v>25.920722990518801</v>
+      </c>
+      <c r="G3" s="8">
+        <v>40498</v>
+      </c>
+      <c r="I3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E4" s="12">
+        <v>-21.170734046437001</v>
+      </c>
+      <c r="F4" s="12">
+        <v>27.5142387604559</v>
+      </c>
+      <c r="G4" s="15">
+        <v>38058</v>
+      </c>
+      <c r="H4" s="15">
+        <v>44168</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="E5" s="12">
+        <v>-21.168105973236401</v>
+      </c>
+      <c r="F5" s="12">
+        <v>27.5115401394225</v>
+      </c>
+      <c r="G5" s="15">
+        <v>40470</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E6" s="12">
+        <v>-24.599938298110601</v>
+      </c>
+      <c r="F6" s="12">
+        <v>24.7287120125049</v>
+      </c>
+      <c r="G6" s="15">
+        <v>40683</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="12">
+        <v>-25.225047877555301</v>
+      </c>
+      <c r="F7" s="12">
+        <v>25.6700058611721</v>
+      </c>
+      <c r="G7" s="15">
+        <v>44160</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D8" t="s">
+        <v>319</v>
+      </c>
+      <c r="E8">
+        <v>-24.6041250172022</v>
+      </c>
+      <c r="F8">
+        <v>25.931394798041001</v>
+      </c>
+      <c r="G8" s="20">
+        <v>44160</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" s="12">
+        <v>-21.975296693519699</v>
+      </c>
+      <c r="F9" s="12">
+        <v>27.844779439437801</v>
+      </c>
+      <c r="G9" s="15">
+        <v>40436</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>320</v>
+      </c>
+      <c r="E10">
+        <v>-24.674451490875999</v>
+      </c>
+      <c r="F10">
+        <v>25.934566275306299</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>313</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>315</v>
+      </c>
+      <c r="E12">
+        <v>-24.642668216974201</v>
+      </c>
+      <c r="F12">
+        <v>25.8854336522826</v>
+      </c>
+      <c r="G12" s="8">
+        <v>37691</v>
+      </c>
+      <c r="H12" s="8">
+        <v>44168</v>
+      </c>
+      <c r="I12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-24.680957355861299</v>
+      </c>
+      <c r="F13" s="1">
+        <v>25.876790287399501</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4029,67 +4700,70 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>323</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>324</v>
       </c>
       <c r="E3">
-        <v>-24.634474726892702</v>
+        <v>-24.604366626171501</v>
       </c>
       <c r="F3">
-        <v>25.873020020798201</v>
+        <v>25.926403997163</v>
+      </c>
+      <c r="G3" s="4">
+        <v>44294</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E4">
-        <v>-23.028580099316802</v>
+        <v>-24.634474726892702</v>
       </c>
       <c r="F4">
-        <v>26.850759675338299</v>
+        <v>25.873020020798201</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E5">
-        <v>-22.479433133400399</v>
+        <v>-23.028580099316802</v>
       </c>
       <c r="F5">
-        <v>27.068283009383599</v>
+        <v>26.850759675338299</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -4098,153 +4772,1083 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6">
-        <v>-21.145645148821</v>
+        <v>-22.479433133400399</v>
       </c>
       <c r="F6">
-        <v>27.519202661585201</v>
+        <v>27.068283009383599</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E7">
-        <v>-24.399704295914798</v>
+        <v>-21.145645148821</v>
       </c>
       <c r="F7">
-        <v>26.147223543590702</v>
+        <v>27.519202661585201</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E8">
-        <v>-24.404042927938601</v>
+        <v>-24.399704295914798</v>
       </c>
       <c r="F8">
-        <v>25.524938681816899</v>
+        <v>26.147223543590702</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E9">
-        <v>-24.787556476787401</v>
+        <v>-24.404042927938601</v>
       </c>
       <c r="F9">
-        <v>25.417263926002398</v>
+        <v>25.524938681816899</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E10">
-        <v>-21.695201102433</v>
+        <v>-24.787556476787401</v>
       </c>
       <c r="F10">
-        <v>21.652218852926101</v>
+        <v>25.417263926002398</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E11">
-        <v>-19.987466712691798</v>
+        <v>-21.695201102433</v>
       </c>
       <c r="F11">
-        <v>23.424740327755401</v>
+        <v>21.652218852926101</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
         <v>184</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E12">
-        <v>-19.3555727318174</v>
+        <v>-19.987466712691798</v>
       </c>
       <c r="F12">
-        <v>22.154923000558899</v>
+        <v>23.424740327755401</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13">
+        <v>-19.3555727318174</v>
+      </c>
+      <c r="F13">
+        <v>22.154923000558899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>189</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14">
+        <v>-17.788301885666598</v>
+      </c>
+      <c r="F14">
+        <v>25.184025254705599</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2">
+        <v>-24.550964854001599</v>
+      </c>
+      <c r="F2">
+        <v>25.986879752984599</v>
+      </c>
+      <c r="G2" s="8">
+        <v>42986</v>
+      </c>
+      <c r="I2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E3">
+        <v>-24.602952431146502</v>
+      </c>
+      <c r="F3">
+        <v>25.926457649565901</v>
+      </c>
+      <c r="G3" s="8">
+        <v>41457</v>
+      </c>
+      <c r="I3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="G4" s="9">
+        <v>41457</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5">
+        <v>-22.420644110428899</v>
+      </c>
+      <c r="F5">
+        <v>26.745212818334998</v>
+      </c>
+      <c r="G5" s="8">
+        <v>42887</v>
+      </c>
+      <c r="I5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E6">
+        <v>-19.977496207161899</v>
+      </c>
+      <c r="F6">
+        <v>23.431474454531401</v>
+      </c>
+      <c r="G6" s="8">
+        <v>44679</v>
+      </c>
+      <c r="I6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G7" s="9">
+        <v>41816</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E8">
+        <v>-24.657678802451901</v>
+      </c>
+      <c r="F8">
+        <v>25.9156048259157</v>
+      </c>
+      <c r="G8" s="8">
+        <v>43843</v>
+      </c>
+      <c r="I8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="12">
+        <v>-21.178050244938898</v>
+      </c>
+      <c r="F9" s="12">
+        <v>27.5118386319315</v>
+      </c>
+      <c r="G9" s="15">
+        <v>41457</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>341</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>342</v>
+      </c>
+      <c r="E10">
+        <v>-24.652849367578</v>
+      </c>
+      <c r="F10">
+        <v>25.888804039676199</v>
+      </c>
+      <c r="G10" s="8">
+        <v>43809</v>
+      </c>
+      <c r="I10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E11">
+        <v>-21.6944913145737</v>
+      </c>
+      <c r="F11">
+        <v>21.648740281761398</v>
+      </c>
+      <c r="G11" s="8">
+        <v>41346</v>
+      </c>
+      <c r="I11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>345</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>346</v>
+      </c>
+      <c r="E12">
+        <v>-24.981032255071099</v>
+      </c>
+      <c r="F12">
+        <v>25.342523720644898</v>
+      </c>
+      <c r="G12" s="8">
+        <v>41828</v>
+      </c>
+      <c r="I12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>347</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>190</v>
+        <v>348</v>
       </c>
       <c r="E13">
-        <v>-17.788301885666598</v>
+        <v>-17.795791616463202</v>
       </c>
       <c r="F13">
-        <v>25.184025254705599</v>
+        <v>25.152881625870201</v>
+      </c>
+      <c r="G13" s="8">
+        <v>41457</v>
+      </c>
+      <c r="I13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>349</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E14">
+        <v>-24.406570867149799</v>
+      </c>
+      <c r="F14">
+        <v>26.106743895209299</v>
+      </c>
+      <c r="G14" s="8">
+        <v>43412</v>
+      </c>
+      <c r="I14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>351</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>352</v>
+      </c>
+      <c r="E15">
+        <v>-24.6781211962486</v>
+      </c>
+      <c r="F15">
+        <v>25.8819375849822</v>
+      </c>
+      <c r="G15" s="8">
+        <v>41541</v>
+      </c>
+      <c r="I15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>354</v>
+      </c>
+      <c r="E16">
+        <v>-24.613963685999199</v>
+      </c>
+      <c r="F16">
+        <v>25.869007137633499</v>
+      </c>
+      <c r="G16" s="8">
+        <v>43809</v>
+      </c>
+      <c r="I16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G17" s="9">
+        <v>43811</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>357</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>358</v>
+      </c>
+      <c r="E18">
+        <v>-21.413243244560601</v>
+      </c>
+      <c r="F18">
+        <v>25.583340499532699</v>
+      </c>
+      <c r="G18" s="8">
+        <v>41453</v>
+      </c>
+      <c r="I18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" t="s">
+        <v>360</v>
+      </c>
+      <c r="E19">
+        <v>-25.229148518766301</v>
+      </c>
+      <c r="F19">
+        <v>25.672383018843998</v>
+      </c>
+      <c r="G19" s="8">
+        <v>44432</v>
+      </c>
+      <c r="I19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>362</v>
+      </c>
+      <c r="E20">
+        <v>-24.407997625170101</v>
+      </c>
+      <c r="F20">
+        <v>25.503518197158801</v>
+      </c>
+      <c r="G20" s="8">
+        <v>41457</v>
+      </c>
+      <c r="I20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G21" s="9">
+        <v>34600</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="E22" s="12">
+        <v>-23.113349247105901</v>
+      </c>
+      <c r="F22" s="12">
+        <v>26.833760499323301</v>
+      </c>
+      <c r="G22" s="15">
+        <v>41828</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>367</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>368</v>
+      </c>
+      <c r="E23">
+        <v>-21.184593387552699</v>
+      </c>
+      <c r="F23">
+        <v>27.533408925929098</v>
+      </c>
+      <c r="G23" s="8">
+        <v>41453</v>
+      </c>
+      <c r="I23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>369</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>370</v>
+      </c>
+      <c r="E24">
+        <v>-24.403519967497601</v>
+      </c>
+      <c r="F24">
+        <v>25.525847010652299</v>
+      </c>
+      <c r="G24" s="8">
+        <v>41473</v>
+      </c>
+      <c r="I24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>371</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>372</v>
+      </c>
+      <c r="E25">
+        <v>-21.1701991457148</v>
+      </c>
+      <c r="F25">
+        <v>27.5108911181267</v>
+      </c>
+      <c r="G25" s="8">
+        <v>41453</v>
+      </c>
+      <c r="I25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>390</v>
+      </c>
+      <c r="D26" t="s">
+        <v>374</v>
+      </c>
+      <c r="E26">
+        <v>-21.331330858872398</v>
+      </c>
+      <c r="F26">
+        <v>25.367230868260901</v>
+      </c>
+      <c r="G26" s="8">
+        <v>41453</v>
+      </c>
+      <c r="I26" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>375</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>376</v>
+      </c>
+      <c r="E27">
+        <v>-22.541881124260801</v>
+      </c>
+      <c r="F27">
+        <v>27.087916137820599</v>
+      </c>
+      <c r="G27" s="8">
+        <v>43033</v>
+      </c>
+      <c r="I27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>377</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>378</v>
+      </c>
+      <c r="E28">
+        <v>-22.554405719069401</v>
+      </c>
+      <c r="F28">
+        <v>27.134350537688899</v>
+      </c>
+      <c r="G28" s="8">
+        <v>41457</v>
+      </c>
+      <c r="I28" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>379</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>380</v>
+      </c>
+      <c r="E29">
+        <v>-24.611966816743902</v>
+      </c>
+      <c r="F29">
+        <v>25.883310875921001</v>
+      </c>
+      <c r="G29" s="8">
+        <v>43809</v>
+      </c>
+      <c r="I29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>381</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" t="s">
+        <v>382</v>
+      </c>
+      <c r="E30">
+        <v>-24.651913275633</v>
+      </c>
+      <c r="F30">
+        <v>25.902536949064299</v>
+      </c>
+      <c r="G30" s="8">
+        <v>41807</v>
+      </c>
+      <c r="I30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>394</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>393</v>
+      </c>
+      <c r="E31">
+        <v>-24.392624770567402</v>
+      </c>
+      <c r="F31">
+        <v>26.144379052838399</v>
+      </c>
+      <c r="G31" s="8">
+        <v>41828</v>
+      </c>
+      <c r="I31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>383</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>384</v>
+      </c>
+      <c r="E32">
+        <v>-22.387782268715998</v>
+      </c>
+      <c r="F32">
+        <v>26.7039865754126</v>
+      </c>
+      <c r="G32" s="8">
+        <v>41452</v>
+      </c>
+      <c r="I32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" t="s">
+        <v>392</v>
+      </c>
+      <c r="E33">
+        <v>-24.6707578180608</v>
+      </c>
+      <c r="F33">
+        <v>25.933551811757201</v>
+      </c>
+      <c r="G33" s="8">
+        <v>41828</v>
+      </c>
+      <c r="I33" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>386</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" t="s">
+        <v>387</v>
+      </c>
+      <c r="E34">
+        <v>-24.6238272544003</v>
+      </c>
+      <c r="F34">
+        <v>25.909746726493001</v>
+      </c>
+      <c r="G34" s="8">
+        <v>43809</v>
+      </c>
+      <c r="I34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>388</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>389</v>
+      </c>
+      <c r="E35">
+        <v>-20.4907569109651</v>
+      </c>
+      <c r="F35">
+        <v>27.0404361346868</v>
+      </c>
+      <c r="G35" s="8">
+        <v>42550</v>
+      </c>
+      <c r="I35" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>